<commit_message>
added spring semester exam results
</commit_message>
<xml_diff>
--- a/admin/XDASI2021_all_grades.xlsx
+++ b/admin/XDASI2021_all_grades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kcg1/code/kriscgun/xdasi-bio-2021/homework_graded/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsierieb/Documents/GitHub/xdasi-bio-2021/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F859E86B-2137-8649-BF42-4CE79CF5B3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75249ED3-127E-6A47-915C-FE2DD28FD424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160" xr2:uid="{B933EA44-64D6-EE45-9B5A-B25C9609ED6C}"/>
   </bookViews>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -210,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,6 +285,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -348,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -366,12 +374,16 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -381,12 +393,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1372,8 +1381,8 @@
   <dimension ref="A1:AF17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AG8" sqref="AG8"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1432,18 +1441,18 @@
       <c r="N1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="25"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="29"/>
       <c r="Y1" s="13" t="s">
         <v>42</v>
       </c>
@@ -1513,50 +1522,50 @@
         <v>95</v>
       </c>
       <c r="O2" s="8">
-        <f>LARGE(C2:N2,1)</f>
+        <f t="shared" ref="O2:O16" si="0">LARGE(C2:N2,1)</f>
         <v>110</v>
       </c>
       <c r="P2" s="8">
-        <f>LARGE(C2:N2,2)</f>
+        <f t="shared" ref="P2:P16" si="1">LARGE(C2:N2,2)</f>
         <v>109</v>
       </c>
       <c r="Q2" s="8">
-        <f>LARGE(C2:N2,3)</f>
+        <f t="shared" ref="Q2:Q16" si="2">LARGE(C2:N2,3)</f>
         <v>100</v>
       </c>
       <c r="R2" s="8">
-        <f>LARGE(C2:N2,4)</f>
+        <f t="shared" ref="R2:R16" si="3">LARGE(C2:N2,4)</f>
         <v>100</v>
       </c>
       <c r="S2" s="8">
-        <f>LARGE(C2:N2,5)</f>
+        <f t="shared" ref="S2:S16" si="4">LARGE(C2:N2,5)</f>
         <v>99</v>
       </c>
       <c r="T2" s="8">
-        <f>LARGE(C2:N2,6)</f>
+        <f t="shared" ref="T2:T16" si="5">LARGE(C2:N2,6)</f>
         <v>99</v>
       </c>
       <c r="U2" s="8">
-        <f>LARGE(C2:N2,7)</f>
+        <f t="shared" ref="U2:U16" si="6">LARGE(C2:N2,7)</f>
         <v>99</v>
       </c>
       <c r="V2" s="8">
-        <f>LARGE(C2:N2,8)</f>
+        <f t="shared" ref="V2:V16" si="7">LARGE(C2:N2,8)</f>
         <v>99</v>
       </c>
       <c r="W2" s="8">
-        <f>LARGE(C2:N2,9)</f>
+        <f t="shared" ref="W2:W16" si="8">LARGE(C2:N2,9)</f>
         <v>99</v>
       </c>
       <c r="X2" s="8">
-        <f>LARGE(C2:N2,10)</f>
+        <f t="shared" ref="X2:X16" si="9">LARGE(C2:N2,10)</f>
         <v>97</v>
       </c>
-      <c r="Y2" s="20">
-        <f>IF(ROUND(AVERAGE(O2:X2),0)&gt;100,100,ROUND(AVERAGE(O2:X2),0))</f>
-        <v>100</v>
-      </c>
-      <c r="Z2" s="18">
+      <c r="Y2" s="18">
+        <f t="shared" ref="Y2:Y16" si="10">IF(ROUND(AVERAGE(O2:X2),0)&gt;100,100,ROUND(AVERAGE(O2:X2),0))</f>
+        <v>100</v>
+      </c>
+      <c r="Z2" s="17">
         <v>100</v>
       </c>
       <c r="AA2" s="14">
@@ -1566,14 +1575,14 @@
         <v>100</v>
       </c>
       <c r="AC2" s="10">
-        <f xml:space="preserve"> Y2*0.7 + Z2*0.1 + AA2*0.1 + AB2*0.1</f>
+        <f t="shared" ref="AC2:AC16" si="11" xml:space="preserve"> Y2*0.7 + Z2*0.1 + AA2*0.1 + AB2*0.1</f>
         <v>98.8</v>
       </c>
       <c r="AD2" s="12"/>
-      <c r="AE2" s="26" t="s">
+      <c r="AE2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AF2" s="31" t="s">
+      <c r="AF2" s="26" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1621,50 +1630,50 @@
         <v>100</v>
       </c>
       <c r="O3" s="8">
-        <f>LARGE(C3:N3,1)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="P3" s="8">
-        <f>LARGE(C3:N3,2)</f>
+        <f t="shared" si="1"/>
         <v>99</v>
       </c>
       <c r="Q3" s="8">
-        <f>LARGE(C3:N3,3)</f>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="R3" s="8">
-        <f>LARGE(C3:N3,4)</f>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="S3" s="8">
-        <f>LARGE(C3:N3,5)</f>
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
       <c r="T3" s="8">
-        <f>LARGE(C3:N3,6)</f>
+        <f t="shared" si="5"/>
         <v>98</v>
       </c>
       <c r="U3" s="8">
-        <f>LARGE(C3:N3,7)</f>
+        <f t="shared" si="6"/>
         <v>98</v>
       </c>
       <c r="V3" s="8">
-        <f>LARGE(C3:N3,8)</f>
+        <f t="shared" si="7"/>
         <v>98</v>
       </c>
       <c r="W3" s="8">
-        <f>LARGE(C3:N3,9)</f>
+        <f t="shared" si="8"/>
         <v>97</v>
       </c>
       <c r="X3" s="8">
-        <f>LARGE(C3:N3,10)</f>
+        <f t="shared" si="9"/>
         <v>97</v>
       </c>
-      <c r="Y3" s="20">
-        <f>IF(ROUND(AVERAGE(O3:X3),0)&gt;100,100,ROUND(AVERAGE(O3:X3),0))</f>
-        <v>98</v>
-      </c>
-      <c r="Z3" s="18">
+      <c r="Y3" s="18">
+        <f t="shared" si="10"/>
+        <v>98</v>
+      </c>
+      <c r="Z3" s="17">
         <v>99</v>
       </c>
       <c r="AA3" s="14">
@@ -1674,14 +1683,14 @@
         <v>100</v>
       </c>
       <c r="AC3" s="10">
-        <f xml:space="preserve"> Y3*0.7 + Z3*0.1 + AA3*0.1 + AB3*0.1</f>
+        <f t="shared" si="11"/>
         <v>95.1</v>
       </c>
       <c r="AD3" s="12"/>
-      <c r="AE3" s="27" t="s">
+      <c r="AE3" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="AF3" s="29" t="s">
+      <c r="AF3" s="24" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1729,50 +1738,50 @@
         <v>95</v>
       </c>
       <c r="O4" s="8">
-        <f>LARGE(C4:N4,1)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
       <c r="P4" s="8">
-        <f>LARGE(C4:N4,2)</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="Q4" s="8">
-        <f>LARGE(C4:N4,3)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="R4" s="8">
-        <f>LARGE(C4:N4,4)</f>
+        <f t="shared" si="3"/>
         <v>99</v>
       </c>
       <c r="S4" s="8">
-        <f>LARGE(C4:N4,5)</f>
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
       <c r="T4" s="8">
-        <f>LARGE(C4:N4,6)</f>
+        <f t="shared" si="5"/>
         <v>99</v>
       </c>
       <c r="U4" s="8">
-        <f>LARGE(C4:N4,7)</f>
+        <f t="shared" si="6"/>
         <v>99</v>
       </c>
       <c r="V4" s="8">
-        <f>LARGE(C4:N4,8)</f>
+        <f t="shared" si="7"/>
         <v>98</v>
       </c>
       <c r="W4" s="8">
-        <f>LARGE(C4:N4,9)</f>
+        <f t="shared" si="8"/>
         <v>98</v>
       </c>
       <c r="X4" s="8">
-        <f>LARGE(C4:N4,10)</f>
+        <f t="shared" si="9"/>
         <v>95</v>
       </c>
-      <c r="Y4" s="20">
-        <f>IF(ROUND(AVERAGE(O4:X4),0)&gt;100,100,ROUND(AVERAGE(O4:X4),0))</f>
-        <v>99</v>
-      </c>
-      <c r="Z4" s="18">
+      <c r="Y4" s="18">
+        <f t="shared" si="10"/>
+        <v>99</v>
+      </c>
+      <c r="Z4" s="17">
         <v>100</v>
       </c>
       <c r="AA4" s="14">
@@ -1782,14 +1791,14 @@
         <v>100</v>
       </c>
       <c r="AC4" s="10">
-        <f xml:space="preserve"> Y4*0.7 + Z4*0.1 + AA4*0.1 + AB4*0.1</f>
+        <f t="shared" si="11"/>
         <v>97.899999999999991</v>
       </c>
       <c r="AD4" s="12"/>
-      <c r="AE4" s="26" t="s">
+      <c r="AE4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AF4" s="31" t="s">
+      <c r="AF4" s="26" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1837,50 +1846,50 @@
         <v>89</v>
       </c>
       <c r="O5" s="8">
-        <f>LARGE(C5:N5,1)</f>
+        <f t="shared" si="0"/>
         <v>109</v>
       </c>
       <c r="P5" s="8">
-        <f>LARGE(C5:N5,2)</f>
+        <f t="shared" si="1"/>
         <v>101</v>
       </c>
       <c r="Q5" s="8">
-        <f>LARGE(C5:N5,3)</f>
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="R5" s="8">
-        <f>LARGE(C5:N5,4)</f>
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="S5" s="8">
-        <f>LARGE(C5:N5,5)</f>
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
       <c r="T5" s="8">
-        <f>LARGE(C5:N5,6)</f>
+        <f t="shared" si="5"/>
         <v>94</v>
       </c>
       <c r="U5" s="8">
-        <f>LARGE(C5:N5,7)</f>
+        <f t="shared" si="6"/>
         <v>94</v>
       </c>
       <c r="V5" s="8">
-        <f>LARGE(C5:N5,8)</f>
+        <f t="shared" si="7"/>
         <v>93</v>
       </c>
       <c r="W5" s="8">
-        <f>LARGE(C5:N5,9)</f>
+        <f t="shared" si="8"/>
         <v>93</v>
       </c>
       <c r="X5" s="8">
-        <f>LARGE(C5:N5,10)</f>
+        <f t="shared" si="9"/>
         <v>93</v>
       </c>
-      <c r="Y5" s="20">
-        <f>IF(ROUND(AVERAGE(O5:X5),0)&gt;100,100,ROUND(AVERAGE(O5:X5),0))</f>
+      <c r="Y5" s="18">
+        <f t="shared" si="10"/>
         <v>97</v>
       </c>
-      <c r="Z5" s="18">
+      <c r="Z5" s="17">
         <v>87</v>
       </c>
       <c r="AA5" s="14">
@@ -1890,14 +1899,14 @@
         <v>100</v>
       </c>
       <c r="AC5" s="10">
-        <f xml:space="preserve"> Y5*0.7 + Z5*0.1 + AA5*0.1 + AB5*0.1</f>
+        <f t="shared" si="11"/>
         <v>93.699999999999989</v>
       </c>
       <c r="AD5" s="12"/>
-      <c r="AE5" s="28" t="s">
+      <c r="AE5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AF5" s="30" t="s">
+      <c r="AF5" s="25" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1945,50 +1954,50 @@
         <v>86</v>
       </c>
       <c r="O6" s="8">
-        <f>LARGE(C6:N6,1)</f>
+        <f t="shared" si="0"/>
         <v>99</v>
       </c>
       <c r="P6" s="8">
-        <f>LARGE(C6:N6,2)</f>
+        <f t="shared" si="1"/>
         <v>99</v>
       </c>
       <c r="Q6" s="8">
-        <f>LARGE(C6:N6,3)</f>
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="R6" s="8">
-        <f>LARGE(C6:N6,4)</f>
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="S6" s="8">
-        <f>LARGE(C6:N6,5)</f>
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
       <c r="T6" s="8">
-        <f>LARGE(C6:N6,6)</f>
+        <f t="shared" si="5"/>
         <v>94</v>
       </c>
       <c r="U6" s="8">
-        <f>LARGE(C6:N6,7)</f>
+        <f t="shared" si="6"/>
         <v>93</v>
       </c>
       <c r="V6" s="8">
-        <f>LARGE(C6:N6,8)</f>
+        <f t="shared" si="7"/>
         <v>89</v>
       </c>
       <c r="W6" s="8">
-        <f>LARGE(C6:N6,9)</f>
+        <f t="shared" si="8"/>
         <v>86</v>
       </c>
       <c r="X6" s="8">
-        <f>LARGE(C6:N6,10)</f>
+        <f t="shared" si="9"/>
         <v>85</v>
       </c>
-      <c r="Y6" s="20">
-        <f>IF(ROUND(AVERAGE(O6:X6),0)&gt;100,100,ROUND(AVERAGE(O6:X6),0))</f>
+      <c r="Y6" s="18">
+        <f t="shared" si="10"/>
         <v>94</v>
       </c>
-      <c r="Z6" s="18">
+      <c r="Z6" s="17">
         <v>96</v>
       </c>
       <c r="AA6" s="14">
@@ -1998,14 +2007,14 @@
         <v>100</v>
       </c>
       <c r="AC6" s="10">
-        <f xml:space="preserve"> Y6*0.7 + Z6*0.1 + AA6*0.1 + AB6*0.1</f>
+        <f t="shared" si="11"/>
         <v>91.7</v>
       </c>
       <c r="AD6" s="12"/>
-      <c r="AE6" s="28" t="s">
+      <c r="AE6" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AF6" s="30" t="s">
+      <c r="AF6" s="25" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2053,50 +2062,50 @@
         <v>100</v>
       </c>
       <c r="O7" s="8">
-        <f>LARGE(C7:N7,1)</f>
+        <f t="shared" si="0"/>
         <v>109</v>
       </c>
       <c r="P7" s="8">
-        <f>LARGE(C7:N7,2)</f>
+        <f t="shared" si="1"/>
         <v>103</v>
       </c>
       <c r="Q7" s="8">
-        <f>LARGE(C7:N7,3)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="R7" s="8">
-        <f>LARGE(C7:N7,4)</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="S7" s="8">
-        <f>LARGE(C7:N7,5)</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="T7" s="8">
-        <f>LARGE(C7:N7,6)</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="U7" s="8">
-        <f>LARGE(C7:N7,7)</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="V7" s="8">
-        <f>LARGE(C7:N7,8)</f>
+        <f t="shared" si="7"/>
         <v>99</v>
       </c>
       <c r="W7" s="8">
-        <f>LARGE(C7:N7,9)</f>
+        <f t="shared" si="8"/>
         <v>99</v>
       </c>
       <c r="X7" s="8">
-        <f>LARGE(C7:N7,10)</f>
+        <f t="shared" si="9"/>
         <v>97</v>
       </c>
-      <c r="Y7" s="20">
-        <f>IF(ROUND(AVERAGE(O7:X7),0)&gt;100,100,ROUND(AVERAGE(O7:X7),0))</f>
-        <v>100</v>
-      </c>
-      <c r="Z7" s="18">
+      <c r="Y7" s="18">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="Z7" s="17">
         <v>100</v>
       </c>
       <c r="AA7" s="14">
@@ -2106,14 +2115,14 @@
         <v>100</v>
       </c>
       <c r="AC7" s="10">
-        <f xml:space="preserve"> Y7*0.7 + Z7*0.1 + AA7*0.1 + AB7*0.1</f>
+        <f t="shared" si="11"/>
         <v>97.3</v>
       </c>
       <c r="AD7" s="12"/>
-      <c r="AE7" s="26" t="s">
+      <c r="AE7" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AF7" s="29" t="s">
+      <c r="AF7" s="24" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2161,50 +2170,50 @@
         <v>100</v>
       </c>
       <c r="O8" s="8">
-        <f>LARGE(C8:N8,1)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="P8" s="8">
-        <f>LARGE(C8:N8,2)</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="Q8" s="8">
-        <f>LARGE(C8:N8,3)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="R8" s="8">
-        <f>LARGE(C8:N8,4)</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="S8" s="8">
-        <f>LARGE(C8:N8,5)</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="T8" s="8">
-        <f>LARGE(C8:N8,6)</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="U8" s="8">
-        <f>LARGE(C8:N8,7)</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="V8" s="8">
-        <f>LARGE(C8:N8,8)</f>
+        <f t="shared" si="7"/>
         <v>99</v>
       </c>
       <c r="W8" s="8">
-        <f>LARGE(C8:N8,9)</f>
+        <f t="shared" si="8"/>
         <v>98</v>
       </c>
       <c r="X8" s="8">
-        <f>LARGE(C8:N8,10)</f>
+        <f t="shared" si="9"/>
         <v>93</v>
       </c>
-      <c r="Y8" s="20">
-        <f>IF(ROUND(AVERAGE(O8:X8),0)&gt;100,100,ROUND(AVERAGE(O8:X8),0))</f>
-        <v>99</v>
-      </c>
-      <c r="Z8" s="18">
+      <c r="Y8" s="18">
+        <f t="shared" si="10"/>
+        <v>99</v>
+      </c>
+      <c r="Z8" s="17">
         <v>93</v>
       </c>
       <c r="AA8" s="14">
@@ -2214,14 +2223,14 @@
         <v>100</v>
       </c>
       <c r="AC8" s="10">
-        <f xml:space="preserve"> Y8*0.7 + Z8*0.1 + AA8*0.1 + AB8*0.1</f>
+        <f t="shared" si="11"/>
         <v>97.899999999999991</v>
       </c>
       <c r="AD8" s="12"/>
-      <c r="AE8" s="26" t="s">
+      <c r="AE8" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AF8" s="31" t="s">
+      <c r="AF8" s="26" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2269,50 +2278,50 @@
         <v>100</v>
       </c>
       <c r="O9" s="8">
-        <f>LARGE(C9:N9,1)</f>
+        <f t="shared" si="0"/>
         <v>109</v>
       </c>
       <c r="P9" s="8">
-        <f>LARGE(C9:N9,2)</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="Q9" s="8">
-        <f>LARGE(C9:N9,3)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="R9" s="8">
-        <f>LARGE(C9:N9,4)</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="S9" s="8">
-        <f>LARGE(C9:N9,5)</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="T9" s="8">
-        <f>LARGE(C9:N9,6)</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="U9" s="8">
-        <f>LARGE(C9:N9,7)</f>
+        <f t="shared" si="6"/>
         <v>99</v>
       </c>
       <c r="V9" s="8">
-        <f>LARGE(C9:N9,8)</f>
+        <f t="shared" si="7"/>
         <v>99</v>
       </c>
       <c r="W9" s="8">
-        <f>LARGE(C9:N9,9)</f>
+        <f t="shared" si="8"/>
         <v>99</v>
       </c>
       <c r="X9" s="8">
-        <f>LARGE(C9:N9,10)</f>
-        <v>99</v>
-      </c>
-      <c r="Y9" s="20">
-        <f>IF(ROUND(AVERAGE(O9:X9),0)&gt;100,100,ROUND(AVERAGE(O9:X9),0))</f>
-        <v>100</v>
-      </c>
-      <c r="Z9" s="18">
+        <f t="shared" si="9"/>
+        <v>99</v>
+      </c>
+      <c r="Y9" s="18">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="Z9" s="17">
         <v>98</v>
       </c>
       <c r="AA9" s="14">
@@ -2322,14 +2331,14 @@
         <v>100</v>
       </c>
       <c r="AC9" s="10">
-        <f xml:space="preserve"> Y9*0.7 + Z9*0.1 + AA9*0.1 + AB9*0.1</f>
+        <f t="shared" si="11"/>
         <v>98.899999999999991</v>
       </c>
       <c r="AD9" s="12"/>
-      <c r="AE9" s="26" t="s">
+      <c r="AE9" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AF9" s="31" t="s">
+      <c r="AF9" s="26" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2377,63 +2386,65 @@
         <v>100</v>
       </c>
       <c r="O10" s="8">
-        <f>LARGE(C10:N10,1)</f>
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="P10" s="8">
-        <f>LARGE(C10:N10,2)</f>
+        <f t="shared" si="1"/>
         <v>109</v>
       </c>
       <c r="Q10" s="8">
-        <f>LARGE(C10:N10,3)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="R10" s="8">
-        <f>LARGE(C10:N10,4)</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="S10" s="8">
-        <f>LARGE(C10:N10,5)</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="T10" s="8">
-        <f>LARGE(C10:N10,6)</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="U10" s="8">
-        <f>LARGE(C10:N10,7)</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="V10" s="8">
-        <f>LARGE(C10:N10,8)</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="W10" s="8">
-        <f>LARGE(C10:N10,9)</f>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="X10" s="8">
-        <f>LARGE(C10:N10,10)</f>
-        <v>100</v>
-      </c>
-      <c r="Y10" s="20">
-        <f>IF(ROUND(AVERAGE(O10:X10),0)&gt;100,100,ROUND(AVERAGE(O10:X10),0))</f>
-        <v>100</v>
-      </c>
-      <c r="Z10" s="19"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5">
-        <v>100</v>
-      </c>
-      <c r="AC10" s="5">
-        <f xml:space="preserve"> Y10*0.7 + Z10*0.1 + AA10*0.1 + AB10*0.1</f>
-        <v>80</v>
-      </c>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="17" t="s">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="Y10" s="18">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="Z10" s="30">
+        <v>100</v>
+      </c>
+      <c r="AA10" s="31"/>
+      <c r="AB10" s="31">
+        <v>100</v>
+      </c>
+      <c r="AC10" s="31">
+        <f t="shared" si="11"/>
+        <v>90</v>
+      </c>
+      <c r="AD10" s="31"/>
+      <c r="AE10" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="AF10" s="17" t="s">
+      <c r="AF10" s="32" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2481,50 +2492,50 @@
         <v>100</v>
       </c>
       <c r="O11" s="8">
-        <f>LARGE(C11:N11,1)</f>
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="P11" s="8">
-        <f>LARGE(C11:N11,2)</f>
+        <f t="shared" si="1"/>
         <v>109</v>
       </c>
       <c r="Q11" s="8">
-        <f>LARGE(C11:N11,3)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="R11" s="8">
-        <f>LARGE(C11:N11,4)</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="S11" s="8">
-        <f>LARGE(C11:N11,5)</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="T11" s="8">
-        <f>LARGE(C11:N11,6)</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="U11" s="8">
-        <f>LARGE(C11:N11,7)</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="V11" s="8">
-        <f>LARGE(C11:N11,8)</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="W11" s="8">
-        <f>LARGE(C11:N11,9)</f>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="X11" s="8">
-        <f>LARGE(C11:N11,10)</f>
-        <v>100</v>
-      </c>
-      <c r="Y11" s="20">
-        <f>IF(ROUND(AVERAGE(O11:X11),0)&gt;100,100,ROUND(AVERAGE(O11:X11),0))</f>
-        <v>100</v>
-      </c>
-      <c r="Z11" s="18">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="Y11" s="18">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="Z11" s="17">
         <v>100</v>
       </c>
       <c r="AA11" s="14">
@@ -2534,14 +2545,14 @@
         <v>100</v>
       </c>
       <c r="AC11" s="10">
-        <f xml:space="preserve"> Y11*0.7 + Z11*0.1 + AA11*0.1 + AB11*0.1</f>
+        <f t="shared" si="11"/>
         <v>97.4</v>
       </c>
       <c r="AD11" s="12"/>
-      <c r="AE11" s="26" t="s">
+      <c r="AE11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AF11" s="29" t="s">
+      <c r="AF11" s="24" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2589,50 +2600,50 @@
         <v>100</v>
       </c>
       <c r="O12" s="8">
-        <f>LARGE(C12:N12,1)</f>
+        <f t="shared" si="0"/>
         <v>108</v>
       </c>
       <c r="P12" s="8">
-        <f>LARGE(C12:N12,2)</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="Q12" s="8">
-        <f>LARGE(C12:N12,3)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="R12" s="8">
-        <f>LARGE(C12:N12,4)</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="S12" s="8">
-        <f>LARGE(C12:N12,5)</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="T12" s="8">
-        <f>LARGE(C12:N12,6)</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="U12" s="8">
-        <f>LARGE(C12:N12,7)</f>
+        <f t="shared" si="6"/>
         <v>99</v>
       </c>
       <c r="V12" s="8">
-        <f>LARGE(C12:N12,8)</f>
+        <f t="shared" si="7"/>
         <v>99</v>
       </c>
       <c r="W12" s="8">
-        <f>LARGE(C12:N12,9)</f>
+        <f t="shared" si="8"/>
         <v>98</v>
       </c>
       <c r="X12" s="8">
-        <f>LARGE(C12:N12,10)</f>
-        <v>98</v>
-      </c>
-      <c r="Y12" s="20">
-        <f>IF(ROUND(AVERAGE(O12:X12),0)&gt;100,100,ROUND(AVERAGE(O12:X12),0))</f>
-        <v>100</v>
-      </c>
-      <c r="Z12" s="18">
+        <f t="shared" si="9"/>
+        <v>98</v>
+      </c>
+      <c r="Y12" s="18">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="Z12" s="17">
         <v>98</v>
       </c>
       <c r="AA12" s="14">
@@ -2642,14 +2653,14 @@
         <v>100</v>
       </c>
       <c r="AC12" s="10">
-        <f xml:space="preserve"> Y12*0.7 + Z12*0.1 + AA12*0.1 + AB12*0.1</f>
+        <f t="shared" si="11"/>
         <v>97.1</v>
       </c>
       <c r="AD12" s="12"/>
-      <c r="AE12" s="26" t="s">
+      <c r="AE12" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AF12" s="29" t="s">
+      <c r="AF12" s="24" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2697,63 +2708,65 @@
         <v>90</v>
       </c>
       <c r="O13" s="8">
-        <f>LARGE(C13:N13,1)</f>
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
       <c r="P13" s="8">
-        <f>LARGE(C13:N13,2)</f>
+        <f t="shared" si="1"/>
         <v>99</v>
       </c>
       <c r="Q13" s="8">
-        <f>LARGE(C13:N13,3)</f>
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="R13" s="8">
-        <f>LARGE(C13:N13,4)</f>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="S13" s="8">
-        <f>LARGE(C13:N13,5)</f>
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
       <c r="T13" s="8">
-        <f>LARGE(C13:N13,6)</f>
+        <f t="shared" si="5"/>
         <v>96</v>
       </c>
       <c r="U13" s="8">
-        <f>LARGE(C13:N13,7)</f>
+        <f t="shared" si="6"/>
         <v>96</v>
       </c>
       <c r="V13" s="8">
-        <f>LARGE(C13:N13,8)</f>
+        <f t="shared" si="7"/>
         <v>92</v>
       </c>
       <c r="W13" s="8">
-        <f>LARGE(C13:N13,9)</f>
+        <f t="shared" si="8"/>
         <v>90</v>
       </c>
       <c r="X13" s="8">
-        <f>LARGE(C13:N13,10)</f>
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
-      <c r="Y13" s="20">
-        <f>IF(ROUND(AVERAGE(O13:X13),0)&gt;100,100,ROUND(AVERAGE(O13:X13),0))</f>
+      <c r="Y13" s="18">
+        <f t="shared" si="10"/>
         <v>96</v>
       </c>
-      <c r="Z13" s="19"/>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="5">
-        <v>100</v>
-      </c>
-      <c r="AC13" s="5">
-        <f xml:space="preserve"> Y13*0.7 + Z13*0.1 + AA13*0.1 + AB13*0.1</f>
-        <v>77.199999999999989</v>
-      </c>
-      <c r="AD13" s="5"/>
-      <c r="AE13" s="17" t="s">
+      <c r="Z13" s="30">
+        <v>88</v>
+      </c>
+      <c r="AA13" s="31"/>
+      <c r="AB13" s="31">
+        <v>100</v>
+      </c>
+      <c r="AC13" s="31">
+        <f t="shared" si="11"/>
+        <v>85.999999999999986</v>
+      </c>
+      <c r="AD13" s="31"/>
+      <c r="AE13" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AF13" s="17" t="s">
+      <c r="AF13" s="32" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2801,50 +2814,50 @@
         <v>95</v>
       </c>
       <c r="O14" s="8">
-        <f>LARGE(C14:N14,1)</f>
+        <f t="shared" si="0"/>
         <v>108</v>
       </c>
       <c r="P14" s="8">
-        <f>LARGE(C14:N14,2)</f>
+        <f t="shared" si="1"/>
         <v>107</v>
       </c>
       <c r="Q14" s="8">
-        <f>LARGE(C14:N14,3)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="R14" s="8">
-        <f>LARGE(C14:N14,4)</f>
+        <f t="shared" si="3"/>
         <v>99</v>
       </c>
       <c r="S14" s="8">
-        <f>LARGE(C14:N14,5)</f>
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
       <c r="T14" s="8">
-        <f>LARGE(C14:N14,6)</f>
+        <f t="shared" si="5"/>
         <v>99</v>
       </c>
       <c r="U14" s="8">
-        <f>LARGE(C14:N14,7)</f>
+        <f t="shared" si="6"/>
         <v>99</v>
       </c>
       <c r="V14" s="8">
-        <f>LARGE(C14:N14,8)</f>
+        <f t="shared" si="7"/>
         <v>98</v>
       </c>
       <c r="W14" s="8">
-        <f>LARGE(C14:N14,9)</f>
+        <f t="shared" si="8"/>
         <v>98</v>
       </c>
       <c r="X14" s="8">
-        <f>LARGE(C14:N14,10)</f>
-        <v>98</v>
-      </c>
-      <c r="Y14" s="20">
-        <f>IF(ROUND(AVERAGE(O14:X14),0)&gt;100,100,ROUND(AVERAGE(O14:X14),0))</f>
-        <v>100</v>
-      </c>
-      <c r="Z14" s="18">
+        <f t="shared" si="9"/>
+        <v>98</v>
+      </c>
+      <c r="Y14" s="18">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="Z14" s="17">
         <v>99</v>
       </c>
       <c r="AA14" s="14">
@@ -2854,14 +2867,14 @@
         <v>100</v>
       </c>
       <c r="AC14" s="10">
-        <f xml:space="preserve"> Y14*0.7 + Z14*0.1 + AA14*0.1 + AB14*0.1</f>
+        <f t="shared" si="11"/>
         <v>98.4</v>
       </c>
       <c r="AD14" s="12"/>
-      <c r="AE14" s="26" t="s">
+      <c r="AE14" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AF14" s="31" t="s">
+      <c r="AF14" s="26" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2909,50 +2922,50 @@
         <v>90</v>
       </c>
       <c r="O15" s="8">
-        <f>LARGE(C15:N15,1)</f>
+        <f t="shared" si="0"/>
         <v>108</v>
       </c>
       <c r="P15" s="8">
-        <f>LARGE(C15:N15,2)</f>
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
       <c r="Q15" s="8">
-        <f>LARGE(C15:N15,3)</f>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="R15" s="8">
-        <f>LARGE(C15:N15,4)</f>
+        <f t="shared" si="3"/>
         <v>99</v>
       </c>
       <c r="S15" s="8">
-        <f>LARGE(C15:N15,5)</f>
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
       <c r="T15" s="8">
-        <f>LARGE(C15:N15,6)</f>
+        <f t="shared" si="5"/>
         <v>98</v>
       </c>
       <c r="U15" s="8">
-        <f>LARGE(C15:N15,7)</f>
+        <f t="shared" si="6"/>
         <v>95</v>
       </c>
       <c r="V15" s="8">
-        <f>LARGE(C15:N15,8)</f>
+        <f t="shared" si="7"/>
         <v>93</v>
       </c>
       <c r="W15" s="8">
-        <f>LARGE(C15:N15,9)</f>
+        <f t="shared" si="8"/>
         <v>93</v>
       </c>
       <c r="X15" s="8">
-        <f>LARGE(C15:N15,10)</f>
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
-      <c r="Y15" s="20">
-        <f>IF(ROUND(AVERAGE(O15:X15),0)&gt;100,100,ROUND(AVERAGE(O15:X15),0))</f>
-        <v>98</v>
-      </c>
-      <c r="Z15" s="18">
+      <c r="Y15" s="18">
+        <f t="shared" si="10"/>
+        <v>98</v>
+      </c>
+      <c r="Z15" s="17">
         <v>98</v>
       </c>
       <c r="AA15" s="14">
@@ -2962,14 +2975,14 @@
         <v>100</v>
       </c>
       <c r="AC15" s="10">
-        <f xml:space="preserve"> Y15*0.7 + Z15*0.1 + AA15*0.1 + AB15*0.1</f>
+        <f t="shared" si="11"/>
         <v>96.3</v>
       </c>
       <c r="AD15" s="12"/>
-      <c r="AE15" s="27" t="s">
+      <c r="AE15" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="AF15" s="29" t="s">
+      <c r="AF15" s="24" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3017,50 +3030,50 @@
         <v>100</v>
       </c>
       <c r="O16" s="8">
-        <f>LARGE(C16:N16,1)</f>
+        <f t="shared" si="0"/>
         <v>109</v>
       </c>
       <c r="P16" s="8">
-        <f>LARGE(C16:N16,2)</f>
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
       <c r="Q16" s="8">
-        <f>LARGE(C16:N16,3)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="R16" s="8">
-        <f>LARGE(C16:N16,4)</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="S16" s="8">
-        <f>LARGE(C16:N16,5)</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="T16" s="8">
-        <f>LARGE(C16:N16,6)</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="U16" s="8">
-        <f>LARGE(C16:N16,7)</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="V16" s="8">
-        <f>LARGE(C16:N16,8)</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="W16" s="8">
-        <f>LARGE(C16:N16,9)</f>
+        <f t="shared" si="8"/>
         <v>99</v>
       </c>
       <c r="X16" s="8">
-        <f>LARGE(C16:N16,10)</f>
-        <v>99</v>
-      </c>
-      <c r="Y16" s="20">
-        <f>IF(ROUND(AVERAGE(O16:X16),0)&gt;100,100,ROUND(AVERAGE(O16:X16),0))</f>
-        <v>100</v>
-      </c>
-      <c r="Z16" s="18">
+        <f t="shared" si="9"/>
+        <v>99</v>
+      </c>
+      <c r="Y16" s="18">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="Z16" s="17">
         <v>100</v>
       </c>
       <c r="AA16" s="14">
@@ -3070,14 +3083,14 @@
         <v>100</v>
       </c>
       <c r="AC16" s="10">
-        <f xml:space="preserve"> Y16*0.7 + Z16*0.1 + AA16*0.1 + AB16*0.1</f>
+        <f t="shared" si="11"/>
         <v>97</v>
       </c>
       <c r="AD16" s="12"/>
-      <c r="AE16" s="26" t="s">
+      <c r="AE16" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AF16" s="29" t="s">
+      <c r="AF16" s="24" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3085,19 +3098,19 @@
       <c r="A17" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="Y17" s="21">
+      <c r="Y17" s="19">
         <v>0.7</v>
       </c>
-      <c r="Z17" s="21">
+      <c r="Z17" s="19">
         <v>0.1</v>
       </c>
-      <c r="AA17" s="22">
+      <c r="AA17" s="20">
         <v>0.1</v>
       </c>
-      <c r="AB17" s="22">
+      <c r="AB17" s="20">
         <v>0.1</v>
       </c>
-      <c r="AC17" s="22">
+      <c r="AC17" s="20">
         <f>SUM(Y17:AB17)</f>
         <v>0.99999999999999989</v>
       </c>

</xml_diff>